<commit_message>
incorporated changes based on tracie's feedback
</commit_message>
<xml_diff>
--- a/data/washington/closures/tables/TableSX_wa_closure_species.xlsx
+++ b/data/washington/closures/tables/TableSX_wa_closure_species.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/data/washington/da_sampling/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/data/washington/closures/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A0DEFB-1497-2C48-A977-3F78A5F1A56D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0332B7-A851-8848-9B57-04BC4BC5F393}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21880" yWindow="5440" windowWidth="28040" windowHeight="17440" xr2:uid="{7D87AE43-3AC6-6F4B-A4D6-BDC5D584B226}"/>
+    <workbookView xWindow="13200" yWindow="2660" windowWidth="28040" windowHeight="17440" xr2:uid="{7D87AE43-3AC6-6F4B-A4D6-BDC5D584B226}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,6 +193,98 @@
     </r>
   </si>
   <si>
+    <t>Species name in data</t>
+  </si>
+  <si>
+    <t>Scientific names and component species</t>
+  </si>
+  <si>
+    <t>Crabs</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <r>
+      <t>Dungeness crab (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Metacarcinus magister</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), red rock crab (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancer productus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), Tanner crab (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chionoecetes bairdi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>All species from the above except crabs and razor clams</t>
+  </si>
+  <si>
+    <t>All species from the above except crabs</t>
+  </si>
+  <si>
+    <t>All species from above (incuding crabs)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -243,100 +335,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>), rock scallop (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Crassodoma gigantea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>Species name in data</t>
-  </si>
-  <si>
-    <t>Scientific names and component species</t>
-  </si>
-  <si>
-    <t>Crabs</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <r>
-      <t>Dungeness crab (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Metacarcinus magister</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>), red rock crab (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cancer productus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>), Tanner crab (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Chionoecetes bairdi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>All species from the above except crabs and razor clams</t>
-  </si>
-  <si>
-    <t>All species from the above except crabs</t>
-  </si>
-  <si>
-    <t>All species from above (incuding crabs)</t>
   </si>
 </sst>
 </file>
@@ -736,7 +757,7 @@
   <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,13 +769,13 @@
   <sheetData>
     <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -842,13 +863,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -856,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
@@ -867,7 +888,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>24</v>
@@ -878,10 +899,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -895,10 +916,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,10 +927,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -917,10 +938,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
began work on new CA data
</commit_message>
<xml_diff>
--- a/data/washington/closures/tables/TableSX_wa_closure_species.xlsx
+++ b/data/washington/closures/tables/TableSX_wa_closure_species.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/data/washington/closures/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F12DB7-E133-0A49-B817-68BD398079EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0E5C84-2ACC-DB4C-AD06-BC8E70C15197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13200" yWindow="2660" windowWidth="28040" windowHeight="17440" xr2:uid="{7D87AE43-3AC6-6F4B-A4D6-BDC5D584B226}"/>
   </bookViews>
@@ -757,7 +757,7 @@
   <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>